<commit_message>
Rough draft. Studies 1-3. Need 2-3 comparison
</commit_message>
<xml_diff>
--- a/data/shipibo_colors (2018_02_21).xlsx
+++ b/data/shipibo_colors (2018_02_21).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielle/Documents/repo/amazon_color/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5FB490-C349-9546-A2AD-D4AA2EFE72E9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BF3890-65C1-D444-BEB7-AB00538194B8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="337">
   <si>
     <t>Term (2017 survey)</t>
   </si>
@@ -1453,7 +1453,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2097,7 +2097,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>52</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>187</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>53</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>54</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>258</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>143</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>262</v>
@@ -2248,7 +2248,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>70</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>76</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>78</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>80</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>161</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>82</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>84</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>86</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>88</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>90</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>98</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>100</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>102</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>103</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>144</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>277</v>
@@ -2550,7 +2550,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>202</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>189</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>96</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>191</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>94</v>
       </c>
@@ -2664,6 +2664,9 @@
       </c>
       <c r="C64" s="2" t="s">
         <v>95</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>284</v>

</xml_diff>

<commit_message>
Update terms: naranja as SK and Spanish
</commit_message>
<xml_diff>
--- a/data/shipibo_colors (2018_02_21).xlsx
+++ b/data/shipibo_colors (2018_02_21).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielle/Documents/repo/amazon_color/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BF3890-65C1-D444-BEB7-AB00538194B8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA4A0CC-B41E-6144-A234-D9A802963FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terms" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="338">
   <si>
     <t>Term (2017 survey)</t>
   </si>
@@ -1043,6 +1043,9 @@
   </si>
   <si>
     <t>AHCT - SLT</t>
+  </si>
+  <si>
+    <t>SK/SP</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1455,8 @@
   <dimension ref="A1:AQ98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2387,7 +2390,7 @@
         <v>163</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>210</v>
+        <v>337</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>270</v>
@@ -3822,7 +3825,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F84">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F84">
     <sortCondition ref="A61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>